<commit_message>
Parte de liquidação 'D+x' e tirando a contabilização de sexta-feira no cálculo do P.U. falta abater o DI caso dado o D+1 da compra D+2 (quebra em taxa e abate)
</commit_message>
<xml_diff>
--- a/BondRates/BondRates2.xlsx
+++ b/BondRates/BondRates2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="18">
   <si>
     <t>Data de Vencimento</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>11/02/2022</t>
+  </si>
+  <si>
+    <t>14/02/2022</t>
+  </si>
+  <si>
+    <t>15/02/2022</t>
   </si>
   <si>
     <t>--</t>
@@ -423,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,7 +478,7 @@
         <v>985.150033</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -495,7 +501,7 @@
         <v>957.883417</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -518,7 +524,7 @@
         <v>929.024398</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -541,7 +547,7 @@
         <v>902.7248039999999</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -564,7 +570,7 @@
         <v>877.305224</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -587,7 +593,7 @@
         <v>854.298862</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -610,7 +616,7 @@
         <v>813.03142</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -633,7 +639,7 @@
         <v>793.4352720000001</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -656,7 +662,7 @@
         <v>774.390426</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -679,7 +685,7 @@
         <v>735.962659</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -702,7 +708,7 @@
         <v>699.547474</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -725,7 +731,7 @@
         <v>993.460638</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -748,7 +754,7 @@
         <v>985.120807</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -771,7 +777,7 @@
         <v>967.4454469999999</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -794,7 +800,7 @@
         <v>942.646058</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -817,7 +823,7 @@
         <v>929.266524</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -840,7 +846,7 @@
         <v>908.871612</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -863,7 +869,7 @@
         <v>11340.152285</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -886,7 +892,7 @@
         <v>11339.222364</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -909,7 +915,7 @@
         <v>11337.668715</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -932,7 +938,7 @@
         <v>11332.15723</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -955,7 +961,7 @@
         <v>11325.749845</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -978,7 +984,7 @@
         <v>11320.555894</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1001,7 +1007,7 @@
         <v>11305.745196</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1024,7 +1030,7 @@
         <v>11287.112748</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1047,7 +1053,7 @@
         <v>11263.978121</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1070,7 +1076,7 @@
         <v>11251.877803</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1093,7 +1099,7 @@
         <v>11219.636751</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1116,7 +1122,7 @@
         <v>11203.079615</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1139,7 +1145,7 @@
         <v>11187.66787</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1162,7 +1168,7 @@
         <v>3900.004127</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1185,7 +1191,7 @@
         <v>3884.112977</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1208,7 +1214,7 @@
         <v>3846.206399</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1231,7 +1237,7 @@
         <v>3955.514674</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1254,7 +1260,7 @@
         <v>3935.196839</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1277,7 +1283,7 @@
         <v>4027.224678</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1300,7 +1306,7 @@
         <v>3972.273652</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1323,7 +1329,7 @@
         <v>4034.707792</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1346,7 +1352,7 @@
         <v>4047.584381</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1369,7 +1375,7 @@
         <v>4050.675067</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1392,7 +1398,7 @@
         <v>4004.219621</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1415,7 +1421,7 @@
         <v>4082.228991</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1438,7 +1444,7 @@
         <v>4034.167302</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1461,7 +1467,7 @@
         <v>4104.784908</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1484,7 +1490,7 @@
         <v>4068.092528</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1507,7 +1513,7 @@
         <v>4134.329125</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1530,7 +1536,7 @@
         <v>985.550171</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1553,7 +1559,7 @@
         <v>958.154867</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1576,7 +1582,7 @@
         <v>928.8835780000001</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1599,7 +1605,7 @@
         <v>902.132334</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1622,7 +1628,7 @@
         <v>876.3981649999999</v>
       </c>
       <c r="G52" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1645,7 +1651,7 @@
         <v>852.8957830000001</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1668,7 +1674,7 @@
         <v>810.990407</v>
       </c>
       <c r="G54" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1691,7 +1697,7 @@
         <v>791.857253</v>
       </c>
       <c r="G55" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1714,7 +1720,7 @@
         <v>772.604888</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1737,7 +1743,7 @@
         <v>734.8571030000001</v>
       </c>
       <c r="G57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1760,7 +1766,7 @@
         <v>698.993956</v>
       </c>
       <c r="G58" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1783,7 +1789,7 @@
         <v>992.827346</v>
       </c>
       <c r="G59" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1806,7 +1812,7 @@
         <v>983.94408</v>
       </c>
       <c r="G60" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1829,7 +1835,7 @@
         <v>970.052502</v>
       </c>
       <c r="G61" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1852,7 +1858,7 @@
         <v>947.320751</v>
       </c>
       <c r="G62" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1875,7 +1881,7 @@
         <v>934.126698</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1898,7 +1904,7 @@
         <v>918.409798</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1921,7 +1927,7 @@
         <v>11344.718743</v>
       </c>
       <c r="G65" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1944,7 +1950,7 @@
         <v>11343.867863</v>
       </c>
       <c r="G66" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1967,7 +1973,7 @@
         <v>11342.234175</v>
       </c>
       <c r="G67" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1990,7 +1996,7 @@
         <v>11336.697786</v>
       </c>
       <c r="G68" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2013,7 +2019,7 @@
         <v>11330.299173</v>
       </c>
       <c r="G69" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2036,7 +2042,7 @@
         <v>11325.341382</v>
       </c>
       <c r="G70" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2059,7 +2065,7 @@
         <v>11310.60415</v>
       </c>
       <c r="G71" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2082,7 +2088,7 @@
         <v>11292.383985</v>
       </c>
       <c r="G72" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2105,7 +2111,7 @@
         <v>11269.353515</v>
       </c>
       <c r="G73" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2128,7 +2134,7 @@
         <v>11257.758865</v>
       </c>
       <c r="G74" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2151,7 +2157,7 @@
         <v>11225.311996</v>
       </c>
       <c r="G75" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2174,7 +2180,7 @@
         <v>11208.79359</v>
       </c>
       <c r="G76" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2197,7 +2203,7 @@
         <v>11194.079048</v>
       </c>
       <c r="G77" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2220,7 +2226,7 @@
         <v>3896.735276</v>
       </c>
       <c r="G78" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2231,10 +2237,10 @@
         <v>45000</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E79">
         <v>6.564</v>
@@ -2243,7 +2249,7 @@
         <v>3877.997458</v>
       </c>
       <c r="G79" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2266,7 +2272,7 @@
         <v>3838.995233</v>
       </c>
       <c r="G80" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2289,7 +2295,7 @@
         <v>3944.828502</v>
       </c>
       <c r="G81" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2312,7 +2318,7 @@
         <v>3924.986668</v>
       </c>
       <c r="G82" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2335,7 +2341,7 @@
         <v>4012.980559</v>
       </c>
       <c r="G83" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2358,7 +2364,7 @@
         <v>3960.695879</v>
       </c>
       <c r="G84" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2381,7 +2387,7 @@
         <v>4025.589185</v>
       </c>
       <c r="G85" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2404,7 +2410,7 @@
         <v>4035.003777</v>
       </c>
       <c r="G86" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2427,7 +2433,7 @@
         <v>4037.067145</v>
       </c>
       <c r="G87" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2450,7 +2456,7 @@
         <v>3990.089356</v>
       </c>
       <c r="G88" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2473,7 +2479,7 @@
         <v>4068.51257</v>
       </c>
       <c r="G89" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2496,7 +2502,7 @@
         <v>4019.562779</v>
       </c>
       <c r="G90" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2519,7 +2525,7 @@
         <v>4088.464806</v>
       </c>
       <c r="G91" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2542,7 +2548,7 @@
         <v>4051.986591</v>
       </c>
       <c r="G92" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2565,7 +2571,7 @@
         <v>4116.902738</v>
       </c>
       <c r="G93" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2588,7 +2594,7 @@
         <v>985.941545</v>
       </c>
       <c r="G94" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2611,7 +2617,7 @@
         <v>958.465133</v>
       </c>
       <c r="G95" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2634,7 +2640,7 @@
         <v>928.834795</v>
       </c>
       <c r="G96" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2657,7 +2663,7 @@
         <v>901.876999</v>
       </c>
       <c r="G97" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2680,7 +2686,7 @@
         <v>875.890966</v>
       </c>
       <c r="G98" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2703,7 +2709,7 @@
         <v>852.003783</v>
       </c>
       <c r="G99" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2726,7 +2732,7 @@
         <v>809.818755</v>
       </c>
       <c r="G100" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2749,7 +2755,7 @@
         <v>790.158646</v>
       </c>
       <c r="G101" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2772,7 +2778,7 @@
         <v>770.81173</v>
       </c>
       <c r="G102" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2795,7 +2801,7 @@
         <v>732.514008</v>
       </c>
       <c r="G103" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2818,7 +2824,7 @@
         <v>695.975052</v>
       </c>
       <c r="G104" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2841,7 +2847,7 @@
         <v>992.550968</v>
       </c>
       <c r="G105" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2864,7 +2870,7 @@
         <v>981.332453</v>
       </c>
       <c r="G106" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2887,7 +2893,7 @@
         <v>966.952733</v>
       </c>
       <c r="G107" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2910,7 +2916,7 @@
         <v>943.8893440000001</v>
       </c>
       <c r="G108" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2933,7 +2939,7 @@
         <v>931.057378</v>
       </c>
       <c r="G109" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2956,7 +2962,7 @@
         <v>915.320713</v>
       </c>
       <c r="G110" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2979,7 +2985,7 @@
         <v>11349.298388</v>
       </c>
       <c r="G111" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3002,7 +3008,7 @@
         <v>11348.447167</v>
       </c>
       <c r="G112" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3025,7 +3031,7 @@
         <v>11346.812822</v>
       </c>
       <c r="G113" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3048,7 +3054,7 @@
         <v>11341.228811</v>
       </c>
       <c r="G114" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3071,7 +3077,7 @@
         <v>11334.929774</v>
       </c>
       <c r="G115" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3094,7 +3100,7 @@
         <v>11330.435326</v>
       </c>
       <c r="G116" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3117,7 +3123,7 @@
         <v>11315.646776</v>
       </c>
       <c r="G117" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3140,7 +3146,7 @@
         <v>11297.532789</v>
       </c>
       <c r="G118" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3163,7 +3169,7 @@
         <v>11274.459019</v>
       </c>
       <c r="G119" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3186,7 +3192,7 @@
         <v>11262.973208</v>
       </c>
       <c r="G120" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3209,7 +3215,7 @@
         <v>11230.025272</v>
       </c>
       <c r="G121" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3232,7 +3238,7 @@
         <v>11214.510347</v>
       </c>
       <c r="G122" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3255,7 +3261,7 @@
         <v>11199.01812</v>
       </c>
       <c r="G123" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3278,7 +3284,7 @@
         <v>3900.129968</v>
       </c>
       <c r="G124" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3289,10 +3295,10 @@
         <v>45000</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D125" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E125">
         <v>6.552</v>
@@ -3301,7 +3307,7 @@
         <v>3880.423937</v>
       </c>
       <c r="G125" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3324,7 +3330,7 @@
         <v>3841.617337</v>
       </c>
       <c r="G126" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3347,7 +3353,7 @@
         <v>3947.05888</v>
       </c>
       <c r="G127" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3370,7 +3376,7 @@
         <v>3920.03401</v>
       </c>
       <c r="G128" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3393,7 +3399,7 @@
         <v>4009.718345</v>
       </c>
       <c r="G129" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3416,7 +3422,7 @@
         <v>3958.76826</v>
       </c>
       <c r="G130" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3439,7 +3445,7 @@
         <v>4022.00653</v>
       </c>
       <c r="G131" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3462,7 +3468,7 @@
         <v>4028.910305</v>
       </c>
       <c r="G132" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3485,7 +3491,7 @@
         <v>4031.374034</v>
       </c>
       <c r="G133" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3508,7 +3514,7 @@
         <v>3983.892973</v>
       </c>
       <c r="G134" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3531,7 +3537,7 @@
         <v>4057.30222</v>
       </c>
       <c r="G135" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3554,7 +3560,7 @@
         <v>4006.333096</v>
       </c>
       <c r="G136" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3577,7 +3583,7 @@
         <v>4075.854448</v>
       </c>
       <c r="G137" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3600,7 +3606,7 @@
         <v>4036.994537</v>
       </c>
       <c r="G138" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3623,7 +3629,7 @@
         <v>4101.074359</v>
       </c>
       <c r="G139" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3646,7 +3652,7 @@
         <v>986.3218450000001</v>
       </c>
       <c r="G140" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3669,7 +3675,7 @@
         <v>958.7717280000001</v>
       </c>
       <c r="G141" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3692,7 +3698,7 @@
         <v>928.883598</v>
       </c>
       <c r="G142" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3715,7 +3721,7 @@
         <v>901.47932</v>
       </c>
       <c r="G143" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3738,7 +3744,7 @@
         <v>874.883696</v>
       </c>
       <c r="G144" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3761,7 +3767,7 @@
         <v>850.427821</v>
       </c>
       <c r="G145" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3784,7 +3790,7 @@
         <v>808.046026</v>
       </c>
       <c r="G146" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3807,7 +3813,7 @@
         <v>787.960926</v>
       </c>
       <c r="G147" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3830,7 +3836,7 @@
         <v>769.357333</v>
       </c>
       <c r="G148" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3853,7 +3859,7 @@
         <v>730.686371</v>
       </c>
       <c r="G149" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3876,7 +3882,7 @@
         <v>694.324028</v>
       </c>
       <c r="G150" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3899,7 +3905,7 @@
         <v>992.071106</v>
       </c>
       <c r="G151" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3922,7 +3928,7 @@
         <v>979.4582820000001</v>
       </c>
       <c r="G152" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3945,7 +3951,7 @@
         <v>965.596254</v>
       </c>
       <c r="G153" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3968,7 +3974,7 @@
         <v>942.17594</v>
       </c>
       <c r="G154" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3991,7 +3997,7 @@
         <v>929.986488</v>
       </c>
       <c r="G155" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -4014,7 +4020,7 @@
         <v>912.965433</v>
       </c>
       <c r="G156" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -4037,7 +4043,7 @@
         <v>11353.868529</v>
       </c>
       <c r="G157" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -4060,7 +4066,7 @@
         <v>11353.096445</v>
       </c>
       <c r="G158" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -4083,7 +4089,7 @@
         <v>11351.574985</v>
       </c>
       <c r="G159" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -4106,7 +4112,7 @@
         <v>11345.79571</v>
       </c>
       <c r="G160" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -4129,7 +4135,7 @@
         <v>11339.494143</v>
       </c>
       <c r="G161" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -4152,7 +4158,7 @@
         <v>11335.27039</v>
       </c>
       <c r="G162" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -4175,7 +4181,7 @@
         <v>11321.123088</v>
       </c>
       <c r="G163" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -4198,7 +4204,7 @@
         <v>11302.729324</v>
       </c>
       <c r="G164" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -4221,7 +4227,7 @@
         <v>11279.918786</v>
       </c>
       <c r="G165" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -4244,7 +4250,7 @@
         <v>11268.746278</v>
       </c>
       <c r="G166" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -4267,7 +4273,7 @@
         <v>11234.967607</v>
       </c>
       <c r="G167" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4290,7 +4296,7 @@
         <v>11220.786243</v>
       </c>
       <c r="G168" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4313,7 +4319,7 @@
         <v>11205.162898</v>
       </c>
       <c r="G169" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4336,7 +4342,7 @@
         <v>3902.98147</v>
       </c>
       <c r="G170" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4359,7 +4365,7 @@
         <v>3882.310541</v>
       </c>
       <c r="G171" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4382,7 +4388,7 @@
         <v>3843.303541</v>
       </c>
       <c r="G172" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4405,7 +4411,7 @@
         <v>3944.304284</v>
       </c>
       <c r="G173" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4428,7 +4434,7 @@
         <v>3914.118709</v>
       </c>
       <c r="G174" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4451,7 +4457,7 @@
         <v>4003.856518</v>
       </c>
       <c r="G175" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4474,7 +4480,7 @@
         <v>3952.98097</v>
       </c>
       <c r="G176" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -4497,7 +4503,7 @@
         <v>4016.715383</v>
       </c>
       <c r="G177" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -4520,7 +4526,7 @@
         <v>4020.821383</v>
       </c>
       <c r="G178" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -4543,7 +4549,7 @@
         <v>4027.502203</v>
       </c>
       <c r="G179" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4566,7 +4572,7 @@
         <v>3982.812317</v>
       </c>
       <c r="G180" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4589,7 +4595,7 @@
         <v>4056.552723</v>
       </c>
       <c r="G181" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -4612,7 +4618,7 @@
         <v>4003.555615</v>
       </c>
       <c r="G182" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4635,7 +4641,7 @@
         <v>4071.514104</v>
       </c>
       <c r="G183" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -4658,7 +4664,7 @@
         <v>4033.931635</v>
       </c>
       <c r="G184" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -4681,7 +4687,2123 @@
         <v>4096.949973</v>
       </c>
       <c r="G185" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B186" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C186">
+        <v>11.1117</v>
+      </c>
+      <c r="D186">
+        <v>11.1015</v>
+      </c>
+      <c r="E186">
+        <v>11.1076</v>
+      </c>
+      <c r="F186">
+        <v>986.713948</v>
+      </c>
+      <c r="G186" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B187" s="2">
+        <v>44743</v>
+      </c>
+      <c r="C187">
+        <v>11.859</v>
+      </c>
+      <c r="D187">
+        <v>11.8302</v>
+      </c>
+      <c r="E187">
+        <v>11.847</v>
+      </c>
+      <c r="F187">
+        <v>959.096595</v>
+      </c>
+      <c r="G187" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B188" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C188">
+        <v>12.37</v>
+      </c>
+      <c r="D188">
+        <v>12.3552</v>
+      </c>
+      <c r="E188">
+        <v>12.3625</v>
+      </c>
+      <c r="F188">
+        <v>929.095403</v>
+      </c>
+      <c r="G188" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B189" s="2">
+        <v>44927</v>
+      </c>
+      <c r="C189">
+        <v>12.5069</v>
+      </c>
+      <c r="D189">
+        <v>12.4951</v>
+      </c>
+      <c r="E189">
+        <v>12.5005</v>
+      </c>
+      <c r="F189">
+        <v>901.858404</v>
+      </c>
+      <c r="G189" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7">
+      <c r="A190" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B190" s="2">
+        <v>45017</v>
+      </c>
+      <c r="C190">
+        <v>12.5538</v>
+      </c>
+      <c r="D190">
+        <v>12.5365</v>
+      </c>
+      <c r="E190">
+        <v>12.5452</v>
+      </c>
+      <c r="F190">
+        <v>875.29674</v>
+      </c>
+      <c r="G190" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7">
+      <c r="A191" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B191" s="2">
+        <v>45108</v>
+      </c>
+      <c r="C191">
+        <v>12.491</v>
+      </c>
+      <c r="D191">
+        <v>12.4781</v>
+      </c>
+      <c r="E191">
+        <v>12.4838</v>
+      </c>
+      <c r="F191">
+        <v>851.246589</v>
+      </c>
+      <c r="G191" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7">
+      <c r="A192" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B192" s="2">
+        <v>45292</v>
+      </c>
+      <c r="C192">
+        <v>12.1411</v>
+      </c>
+      <c r="D192">
+        <v>12.1276</v>
+      </c>
+      <c r="E192">
+        <v>12.1338</v>
+      </c>
+      <c r="F192">
+        <v>807.676423</v>
+      </c>
+      <c r="G192" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
+      <c r="A193" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B193" s="2">
+        <v>45383</v>
+      </c>
+      <c r="C193">
+        <v>12.0111</v>
+      </c>
+      <c r="D193">
+        <v>11.9985</v>
+      </c>
+      <c r="E193">
+        <v>12.0036</v>
+      </c>
+      <c r="F193">
+        <v>787.519254</v>
+      </c>
+      <c r="G193" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7">
+      <c r="A194" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B194" s="2">
+        <v>45474</v>
+      </c>
+      <c r="C194">
+        <v>11.8197</v>
+      </c>
+      <c r="D194">
+        <v>11.804</v>
+      </c>
+      <c r="E194">
+        <v>11.8122</v>
+      </c>
+      <c r="F194">
+        <v>768.606487</v>
+      </c>
+      <c r="G194" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7">
+      <c r="A195" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B195" s="2">
+        <v>45658</v>
+      </c>
+      <c r="C195">
+        <v>11.5767</v>
+      </c>
+      <c r="D195">
+        <v>11.5622</v>
+      </c>
+      <c r="E195">
+        <v>11.5692</v>
+      </c>
+      <c r="F195">
+        <v>730.1371</v>
+      </c>
+      <c r="G195" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7">
+      <c r="A196" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B196" s="2">
+        <v>45839</v>
+      </c>
+      <c r="C196">
+        <v>11.5087</v>
+      </c>
+      <c r="D196">
+        <v>11.4975</v>
+      </c>
+      <c r="E196">
+        <v>11.5036</v>
+      </c>
+      <c r="F196">
+        <v>693.816211</v>
+      </c>
+      <c r="G196" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B197" s="2">
+        <v>44927</v>
+      </c>
+      <c r="C197">
+        <v>12.5215</v>
+      </c>
+      <c r="D197">
+        <v>12.5037</v>
+      </c>
+      <c r="E197">
+        <v>12.5126</v>
+      </c>
+      <c r="F197">
+        <v>992.496776</v>
+      </c>
+      <c r="G197" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B198" s="2">
+        <v>45658</v>
+      </c>
+      <c r="C198">
+        <v>11.475</v>
+      </c>
+      <c r="D198">
+        <v>11.449</v>
+      </c>
+      <c r="E198">
+        <v>11.4629</v>
+      </c>
+      <c r="F198">
+        <v>978.852827</v>
+      </c>
+      <c r="G198" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B199" s="2">
+        <v>46388</v>
+      </c>
+      <c r="C199">
+        <v>11.35</v>
+      </c>
+      <c r="D199">
+        <v>11.3277</v>
+      </c>
+      <c r="E199">
+        <v>11.3371</v>
+      </c>
+      <c r="F199">
+        <v>965.654254</v>
+      </c>
+      <c r="G199" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B200" s="2">
+        <v>47119</v>
+      </c>
+      <c r="C200">
+        <v>11.605</v>
+      </c>
+      <c r="D200">
+        <v>11.5915</v>
+      </c>
+      <c r="E200">
+        <v>11.5971</v>
+      </c>
+      <c r="F200">
+        <v>942.2852789999999</v>
+      </c>
+      <c r="G200" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B201" s="2">
+        <v>47849</v>
+      </c>
+      <c r="C201">
+        <v>11.6217</v>
+      </c>
+      <c r="D201">
+        <v>11.5984</v>
+      </c>
+      <c r="E201">
+        <v>11.61</v>
+      </c>
+      <c r="F201">
+        <v>929.406668</v>
+      </c>
+      <c r="G201" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B202" s="2">
+        <v>48580</v>
+      </c>
+      <c r="C202">
+        <v>11.755</v>
+      </c>
+      <c r="D202">
+        <v>11.74</v>
+      </c>
+      <c r="E202">
+        <v>11.7476</v>
+      </c>
+      <c r="F202">
+        <v>911.732387</v>
+      </c>
+      <c r="G202" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7">
+      <c r="A203" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B203" s="2">
+        <v>44621</v>
+      </c>
+      <c r="C203">
+        <v>0.0722</v>
+      </c>
+      <c r="D203">
+        <v>0.0606</v>
+      </c>
+      <c r="E203">
+        <v>0.0653</v>
+      </c>
+      <c r="F203">
+        <v>11358.440509</v>
+      </c>
+      <c r="G203" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7">
+      <c r="A204" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B204" s="2">
+        <v>44805</v>
+      </c>
+      <c r="C204">
+        <v>0.0216</v>
+      </c>
+      <c r="D204">
+        <v>0.0058</v>
+      </c>
+      <c r="E204">
+        <v>0.017</v>
+      </c>
+      <c r="F204">
+        <v>11357.668115</v>
+      </c>
+      <c r="G204" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7">
+      <c r="A205" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B205" s="2">
+        <v>44986</v>
+      </c>
+      <c r="C205">
+        <v>0.0295</v>
+      </c>
+      <c r="D205">
+        <v>0.0133</v>
+      </c>
+      <c r="E205">
+        <v>0.0224</v>
+      </c>
+      <c r="F205">
+        <v>11356.10061</v>
+      </c>
+      <c r="G205" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7">
+      <c r="A206" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B206" s="2">
+        <v>45170</v>
+      </c>
+      <c r="C206">
+        <v>0.0507</v>
+      </c>
+      <c r="D206">
+        <v>0.0418</v>
+      </c>
+      <c r="E206">
+        <v>0.0467</v>
+      </c>
+      <c r="F206">
+        <v>11350.546188</v>
+      </c>
+      <c r="G206" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
+      <c r="A207" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B207" s="2">
+        <v>45352</v>
+      </c>
+      <c r="C207">
+        <v>0.0698</v>
+      </c>
+      <c r="D207">
+        <v>0.0543</v>
+      </c>
+      <c r="E207">
+        <v>0.06320000000000001</v>
+      </c>
+      <c r="F207">
+        <v>11344.185296</v>
+      </c>
+      <c r="G207" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7">
+      <c r="A208" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B208" s="2">
+        <v>45536</v>
+      </c>
+      <c r="C208">
+        <v>0.0701</v>
+      </c>
+      <c r="D208">
+        <v>0.0574</v>
+      </c>
+      <c r="E208">
+        <v>0.0654</v>
+      </c>
+      <c r="F208">
+        <v>11339.914411</v>
+      </c>
+      <c r="G208" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7">
+      <c r="A209" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B209" s="2">
+        <v>45717</v>
+      </c>
+      <c r="C209">
+        <v>0.1017</v>
+      </c>
+      <c r="D209">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="E209">
+        <v>0.09619999999999999</v>
+      </c>
+      <c r="F209">
+        <v>11325.579687</v>
+      </c>
+      <c r="G209" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
+      <c r="A210" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B210" s="2">
+        <v>45901</v>
+      </c>
+      <c r="C210">
+        <v>0.131</v>
+      </c>
+      <c r="D210">
+        <v>0.1179</v>
+      </c>
+      <c r="E210">
+        <v>0.1271</v>
+      </c>
+      <c r="F210">
+        <v>11307.894135</v>
+      </c>
+      <c r="G210" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
+      <c r="A211" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B211" s="2">
+        <v>46082</v>
+      </c>
+      <c r="C211">
+        <v>0.1657</v>
+      </c>
+      <c r="D211">
+        <v>0.1528</v>
+      </c>
+      <c r="E211">
+        <v>0.1616</v>
+      </c>
+      <c r="F211">
+        <v>11285.029</v>
+      </c>
+      <c r="G211" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7">
+      <c r="A212" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B212" s="2">
+        <v>46266</v>
+      </c>
+      <c r="C212">
+        <v>0.17</v>
+      </c>
+      <c r="D212">
+        <v>0.1521</v>
+      </c>
+      <c r="E212">
+        <v>0.165</v>
+      </c>
+      <c r="F212">
+        <v>11274.113255</v>
+      </c>
+      <c r="G212" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="A213" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B213" s="2">
+        <v>46447</v>
+      </c>
+      <c r="C213">
+        <v>0.215</v>
+      </c>
+      <c r="D213">
+        <v>0.2032</v>
+      </c>
+      <c r="E213">
+        <v>0.2101</v>
+      </c>
+      <c r="F213">
+        <v>11239.684926</v>
+      </c>
+      <c r="G213" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
+      <c r="A214" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B214" s="2">
+        <v>46631</v>
+      </c>
+      <c r="C214">
+        <v>0.22</v>
+      </c>
+      <c r="D214">
+        <v>0.2025</v>
+      </c>
+      <c r="E214">
+        <v>0.213</v>
+      </c>
+      <c r="F214">
+        <v>11225.81591</v>
+      </c>
+      <c r="G214" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
+      <c r="A215" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B215" s="2">
+        <v>46813</v>
+      </c>
+      <c r="C215">
+        <v>0.2212</v>
+      </c>
+      <c r="D215">
+        <v>0.2118</v>
+      </c>
+      <c r="E215">
+        <v>0.218</v>
+      </c>
+      <c r="F215">
+        <v>11210.708791</v>
+      </c>
+      <c r="G215" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7">
+      <c r="A216" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B216" s="2">
+        <v>44788</v>
+      </c>
+      <c r="C216">
+        <v>6.8874</v>
+      </c>
+      <c r="D216">
+        <v>6.8533</v>
+      </c>
+      <c r="E216">
+        <v>6.87</v>
+      </c>
+      <c r="F216">
+        <v>3907.944854</v>
+      </c>
+      <c r="G216" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
+      <c r="A217" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B217" s="2">
+        <v>45000</v>
+      </c>
+      <c r="C217">
+        <v>6.47</v>
+      </c>
+      <c r="D217">
+        <v>6.43</v>
+      </c>
+      <c r="E217">
+        <v>6.45</v>
+      </c>
+      <c r="F217">
+        <v>3888.217283</v>
+      </c>
+      <c r="G217" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B218" s="2">
+        <v>45061</v>
+      </c>
+      <c r="C218">
+        <v>6.47</v>
+      </c>
+      <c r="D218">
+        <v>6.4353</v>
+      </c>
+      <c r="E218">
+        <v>6.45</v>
+      </c>
+      <c r="F218">
+        <v>3849.748902</v>
+      </c>
+      <c r="G218" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B219" s="2">
+        <v>45519</v>
+      </c>
+      <c r="C219">
+        <v>5.7294</v>
+      </c>
+      <c r="D219">
+        <v>5.69</v>
+      </c>
+      <c r="E219">
+        <v>5.7092</v>
+      </c>
+      <c r="F219">
+        <v>3949.666875</v>
+      </c>
+      <c r="G219" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B220" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C220">
+        <v>5.5639</v>
+      </c>
+      <c r="D220">
+        <v>5.534</v>
+      </c>
+      <c r="E220">
+        <v>5.55</v>
+      </c>
+      <c r="F220">
+        <v>3918.677292</v>
+      </c>
+      <c r="G220" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B221" s="2">
+        <v>46249</v>
+      </c>
+      <c r="C221">
+        <v>5.4258</v>
+      </c>
+      <c r="D221">
+        <v>5.3922</v>
+      </c>
+      <c r="E221">
+        <v>5.4057</v>
+      </c>
+      <c r="F221">
+        <v>4011.112657</v>
+      </c>
+      <c r="G221" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B222" s="2">
+        <v>46522</v>
+      </c>
+      <c r="C222">
+        <v>5.4626</v>
+      </c>
+      <c r="D222">
+        <v>5.4265</v>
+      </c>
+      <c r="E222">
+        <v>5.4421</v>
+      </c>
+      <c r="F222">
+        <v>3962.974794</v>
+      </c>
+      <c r="G222" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B223" s="2">
+        <v>46980</v>
+      </c>
+      <c r="C223">
+        <v>5.5205</v>
+      </c>
+      <c r="D223">
+        <v>5.4862</v>
+      </c>
+      <c r="E223">
+        <v>5.5018</v>
+      </c>
+      <c r="F223">
+        <v>4025.906429</v>
+      </c>
+      <c r="G223" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7">
+      <c r="A224" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B224" s="2">
+        <v>47710</v>
+      </c>
+      <c r="C224">
+        <v>5.6056</v>
+      </c>
+      <c r="D224">
+        <v>5.5712</v>
+      </c>
+      <c r="E224">
+        <v>5.5892</v>
+      </c>
+      <c r="F224">
+        <v>4030.390661</v>
+      </c>
+      <c r="G224" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7">
+      <c r="A225" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B225" s="2">
+        <v>48441</v>
+      </c>
+      <c r="C225">
+        <v>5.6422</v>
+      </c>
+      <c r="D225">
+        <v>5.6061</v>
+      </c>
+      <c r="E225">
+        <v>5.6233</v>
+      </c>
+      <c r="F225">
+        <v>4037.183681</v>
+      </c>
+      <c r="G225" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7">
+      <c r="A226" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B226" s="2">
+        <v>49444</v>
+      </c>
+      <c r="C226">
+        <v>5.6634</v>
+      </c>
+      <c r="D226">
+        <v>5.6322</v>
+      </c>
+      <c r="E226">
+        <v>5.65</v>
+      </c>
+      <c r="F226">
+        <v>3993.914848</v>
+      </c>
+      <c r="G226" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7">
+      <c r="A227" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B227" s="2">
+        <v>51363</v>
+      </c>
+      <c r="C227">
+        <v>5.7005</v>
+      </c>
+      <c r="D227">
+        <v>5.6572</v>
+      </c>
+      <c r="E227">
+        <v>5.6766</v>
+      </c>
+      <c r="F227">
+        <v>4067.060778</v>
+      </c>
+      <c r="G227" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7">
+      <c r="A228" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B228" s="2">
+        <v>53097</v>
+      </c>
+      <c r="C228">
+        <v>5.7425</v>
+      </c>
+      <c r="D228">
+        <v>5.6946</v>
+      </c>
+      <c r="E228">
+        <v>5.7193</v>
+      </c>
+      <c r="F228">
+        <v>4009.424879</v>
+      </c>
+      <c r="G228" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7">
+      <c r="A229" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B229" s="2">
+        <v>55015</v>
+      </c>
+      <c r="C229">
+        <v>5.7426</v>
+      </c>
+      <c r="D229">
+        <v>5.7012</v>
+      </c>
+      <c r="E229">
+        <v>5.7213</v>
+      </c>
+      <c r="F229">
+        <v>4077.972281</v>
+      </c>
+      <c r="G229" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="A230" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B230" s="2">
+        <v>56749</v>
+      </c>
+      <c r="C230">
+        <v>5.7214</v>
+      </c>
+      <c r="D230">
+        <v>5.6853</v>
+      </c>
+      <c r="E230">
+        <v>5.7057</v>
+      </c>
+      <c r="F230">
+        <v>4040.326834</v>
+      </c>
+      <c r="G230" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
+      <c r="A231" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B231" s="2">
+        <v>58668</v>
+      </c>
+      <c r="C231">
+        <v>5.722</v>
+      </c>
+      <c r="D231">
+        <v>5.6851</v>
+      </c>
+      <c r="E231">
+        <v>5.7048</v>
+      </c>
+      <c r="F231">
+        <v>4104.805282</v>
+      </c>
+      <c r="G231" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="A232" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B232" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C232">
+        <v>11.1068</v>
+      </c>
+      <c r="D232">
+        <v>11.0932</v>
+      </c>
+      <c r="E232">
+        <v>11.1013</v>
+      </c>
+      <c r="F232">
+        <v>987.133339</v>
+      </c>
+      <c r="G232" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7">
+      <c r="A233" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B233" s="2">
+        <v>44743</v>
+      </c>
+      <c r="C233">
+        <v>11.8301</v>
+      </c>
+      <c r="D233">
+        <v>11.805</v>
+      </c>
+      <c r="E233">
+        <v>11.8175</v>
+      </c>
+      <c r="F233">
+        <v>959.616224</v>
+      </c>
+      <c r="G233" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7">
+      <c r="A234" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B234" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C234">
+        <v>12.2935</v>
+      </c>
+      <c r="D234">
+        <v>12.2811</v>
+      </c>
+      <c r="E234">
+        <v>12.2879</v>
+      </c>
+      <c r="F234">
+        <v>929.912387</v>
+      </c>
+      <c r="G234" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7">
+      <c r="A235" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B235" s="2">
+        <v>44927</v>
+      </c>
+      <c r="C235">
+        <v>12.415</v>
+      </c>
+      <c r="D235">
+        <v>12.4018</v>
+      </c>
+      <c r="E235">
+        <v>12.4086</v>
+      </c>
+      <c r="F235">
+        <v>902.923998</v>
+      </c>
+      <c r="G235" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
+      <c r="A236" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B236" s="2">
+        <v>45017</v>
+      </c>
+      <c r="C236">
+        <v>12.4327</v>
+      </c>
+      <c r="D236">
+        <v>12.415</v>
+      </c>
+      <c r="E236">
+        <v>12.425</v>
+      </c>
+      <c r="F236">
+        <v>876.758853</v>
+      </c>
+      <c r="G236" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
+      <c r="A237" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B237" s="2">
+        <v>45108</v>
+      </c>
+      <c r="C237">
+        <v>12.3737</v>
+      </c>
+      <c r="D237">
+        <v>12.3628</v>
+      </c>
+      <c r="E237">
+        <v>12.3686</v>
+      </c>
+      <c r="F237">
+        <v>852.836141</v>
+      </c>
+      <c r="G237" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
+      <c r="A238" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B238" s="2">
+        <v>45292</v>
+      </c>
+      <c r="C238">
+        <v>11.9964</v>
+      </c>
+      <c r="D238">
+        <v>11.9855</v>
+      </c>
+      <c r="E238">
+        <v>11.9908</v>
+      </c>
+      <c r="F238">
+        <v>809.964878</v>
+      </c>
+      <c r="G238" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B239" s="2">
+        <v>45383</v>
+      </c>
+      <c r="C239">
+        <v>11.8658</v>
+      </c>
+      <c r="D239">
+        <v>11.8523</v>
+      </c>
+      <c r="E239">
+        <v>11.8575</v>
+      </c>
+      <c r="F239">
+        <v>790.039452</v>
+      </c>
+      <c r="G239" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="A240" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B240" s="2">
+        <v>45474</v>
+      </c>
+      <c r="C240">
+        <v>11.6937</v>
+      </c>
+      <c r="D240">
+        <v>11.6802</v>
+      </c>
+      <c r="E240">
+        <v>11.6873</v>
+      </c>
+      <c r="F240">
+        <v>770.972159</v>
+      </c>
+      <c r="G240" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7">
+      <c r="A241" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B241" s="2">
+        <v>45658</v>
+      </c>
+      <c r="C241">
+        <v>11.4317</v>
+      </c>
+      <c r="D241">
+        <v>11.4183</v>
+      </c>
+      <c r="E241">
+        <v>11.425</v>
+      </c>
+      <c r="F241">
+        <v>733.169788</v>
+      </c>
+      <c r="G241" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7">
+      <c r="A242" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B242" s="2">
+        <v>45839</v>
+      </c>
+      <c r="C242">
+        <v>11.3789</v>
+      </c>
+      <c r="D242">
+        <v>11.3666</v>
+      </c>
+      <c r="E242">
+        <v>11.3727</v>
+      </c>
+      <c r="F242">
+        <v>696.85543</v>
+      </c>
+      <c r="G242" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
+      <c r="A243" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B243" s="2">
+        <v>44927</v>
+      </c>
+      <c r="C243">
+        <v>12.4262</v>
+      </c>
+      <c r="D243">
+        <v>12.4093</v>
+      </c>
+      <c r="E243">
+        <v>12.4183</v>
+      </c>
+      <c r="F243">
+        <v>993.668574</v>
+      </c>
+      <c r="G243" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7">
+      <c r="A244" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B244" s="2">
+        <v>45658</v>
+      </c>
+      <c r="C244">
+        <v>11.3297</v>
+      </c>
+      <c r="D244">
+        <v>11.3064</v>
+      </c>
+      <c r="E244">
+        <v>11.316</v>
+      </c>
+      <c r="F244">
+        <v>982.551945</v>
+      </c>
+      <c r="G244" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7">
+      <c r="A245" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B245" s="2">
+        <v>46388</v>
+      </c>
+      <c r="C245">
+        <v>11.2084</v>
+      </c>
+      <c r="D245">
+        <v>11.1873</v>
+      </c>
+      <c r="E245">
+        <v>11.1957</v>
+      </c>
+      <c r="F245">
+        <v>970.881114</v>
+      </c>
+      <c r="G245" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="A246" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B246" s="2">
+        <v>47119</v>
+      </c>
+      <c r="C246">
+        <v>11.4627</v>
+      </c>
+      <c r="D246">
+        <v>11.4506</v>
+      </c>
+      <c r="E246">
+        <v>11.4561</v>
+      </c>
+      <c r="F246">
+        <v>948.691623</v>
+      </c>
+      <c r="G246" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="A247" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B247" s="2">
+        <v>47849</v>
+      </c>
+      <c r="C247">
+        <v>11.5228</v>
+      </c>
+      <c r="D247">
+        <v>11.4985</v>
+      </c>
+      <c r="E247">
+        <v>11.51</v>
+      </c>
+      <c r="F247">
+        <v>934.748843</v>
+      </c>
+      <c r="G247" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7">
+      <c r="A248" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B248" s="2">
+        <v>48580</v>
+      </c>
+      <c r="C248">
+        <v>11.6567</v>
+      </c>
+      <c r="D248">
+        <v>11.6395</v>
+      </c>
+      <c r="E248">
+        <v>11.6483</v>
+      </c>
+      <c r="F248">
+        <v>917.506677</v>
+      </c>
+      <c r="G248" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7">
+      <c r="A249" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B249" s="2">
+        <v>44621</v>
+      </c>
+      <c r="C249">
+        <v>0.0926</v>
+      </c>
+      <c r="D249">
+        <v>0.0751</v>
+      </c>
+      <c r="E249">
+        <v>0.0912</v>
+      </c>
+      <c r="F249">
+        <v>11362.923425</v>
+      </c>
+      <c r="G249" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7">
+      <c r="A250" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B250" s="2">
+        <v>44805</v>
+      </c>
+      <c r="C250">
+        <v>0.0248</v>
+      </c>
+      <c r="D250">
+        <v>0.0069</v>
+      </c>
+      <c r="E250">
+        <v>0.0168</v>
+      </c>
+      <c r="F250">
+        <v>11362.25299</v>
+      </c>
+      <c r="G250" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7">
+      <c r="A251" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B251" s="2">
+        <v>44986</v>
+      </c>
+      <c r="C251">
+        <v>0.0274</v>
+      </c>
+      <c r="D251">
+        <v>0.0154</v>
+      </c>
+      <c r="E251">
+        <v>0.022</v>
+      </c>
+      <c r="F251">
+        <v>11360.718945</v>
+      </c>
+      <c r="G251" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B252" s="2">
+        <v>45170</v>
+      </c>
+      <c r="C252">
+        <v>0.0501</v>
+      </c>
+      <c r="D252">
+        <v>0.0415</v>
+      </c>
+      <c r="E252">
+        <v>0.0467</v>
+      </c>
+      <c r="F252">
+        <v>11355.128202</v>
+      </c>
+      <c r="G252" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B253" s="2">
+        <v>45352</v>
+      </c>
+      <c r="C253">
+        <v>0.066</v>
+      </c>
+      <c r="D253">
+        <v>0.0572</v>
+      </c>
+      <c r="E253">
+        <v>0.0633</v>
+      </c>
+      <c r="F253">
+        <v>11348.753392</v>
+      </c>
+      <c r="G253" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B254" s="2">
+        <v>45536</v>
+      </c>
+      <c r="C254">
+        <v>0.06950000000000001</v>
+      </c>
+      <c r="D254">
+        <v>0.0575</v>
+      </c>
+      <c r="E254">
+        <v>0.064</v>
+      </c>
+      <c r="F254">
+        <v>11344.901233</v>
+      </c>
+      <c r="G254" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B255" s="2">
+        <v>45717</v>
+      </c>
+      <c r="C255">
+        <v>0.1004</v>
+      </c>
+      <c r="D255">
+        <v>0.0871</v>
+      </c>
+      <c r="E255">
+        <v>0.09420000000000001</v>
+      </c>
+      <c r="F255">
+        <v>11330.856197</v>
+      </c>
+      <c r="G255" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B256" s="2">
+        <v>45901</v>
+      </c>
+      <c r="C256">
+        <v>0.1306</v>
+      </c>
+      <c r="D256">
+        <v>0.1181</v>
+      </c>
+      <c r="E256">
+        <v>0.1245</v>
+      </c>
+      <c r="F256">
+        <v>11313.527166</v>
+      </c>
+      <c r="G256" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B257" s="2">
+        <v>46082</v>
+      </c>
+      <c r="C257">
+        <v>0.165</v>
+      </c>
+      <c r="D257">
+        <v>0.153</v>
+      </c>
+      <c r="E257">
+        <v>0.1593</v>
+      </c>
+      <c r="F257">
+        <v>11290.675573</v>
+      </c>
+      <c r="G257" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7">
+      <c r="A258" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B258" s="2">
+        <v>46266</v>
+      </c>
+      <c r="C258">
+        <v>0.1692</v>
+      </c>
+      <c r="D258">
+        <v>0.1556</v>
+      </c>
+      <c r="E258">
+        <v>0.1627</v>
+      </c>
+      <c r="F258">
+        <v>11279.88044</v>
+      </c>
+      <c r="G258" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B259" s="2">
+        <v>46447</v>
+      </c>
+      <c r="C259">
+        <v>0.215</v>
+      </c>
+      <c r="D259">
+        <v>0.1995</v>
+      </c>
+      <c r="E259">
+        <v>0.2067</v>
+      </c>
+      <c r="F259">
+        <v>11246.210987</v>
+      </c>
+      <c r="G259" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7">
+      <c r="A260" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B260" s="2">
+        <v>46631</v>
+      </c>
+      <c r="C260">
+        <v>0.2118</v>
+      </c>
+      <c r="D260">
+        <v>0.2032</v>
+      </c>
+      <c r="E260">
+        <v>0.208</v>
+      </c>
+      <c r="F260">
+        <v>11233.518182</v>
+      </c>
+      <c r="G260" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7">
+      <c r="A261" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B261" s="2">
+        <v>46813</v>
+      </c>
+      <c r="C261">
+        <v>0.2146</v>
+      </c>
+      <c r="D261">
+        <v>0.2006</v>
+      </c>
+      <c r="E261">
+        <v>0.2082</v>
+      </c>
+      <c r="F261">
+        <v>11221.904891</v>
+      </c>
+      <c r="G261" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7">
+      <c r="A262" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B262" s="2">
+        <v>44788</v>
+      </c>
+      <c r="C262">
+        <v>6.7737</v>
+      </c>
+      <c r="D262">
+        <v>6.7416</v>
+      </c>
+      <c r="E262">
+        <v>6.7581</v>
+      </c>
+      <c r="F262">
+        <v>3799.274508</v>
+      </c>
+      <c r="G262" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7">
+      <c r="A263" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B263" s="2">
+        <v>45000</v>
+      </c>
+      <c r="C263" t="s">
+        <v>13</v>
+      </c>
+      <c r="D263" t="s">
+        <v>13</v>
+      </c>
+      <c r="E263">
+        <v>6.334</v>
+      </c>
+      <c r="F263">
+        <v>3894.545996</v>
+      </c>
+      <c r="G263" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7">
+      <c r="A264" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B264" s="2">
+        <v>45061</v>
+      </c>
+      <c r="C264">
+        <v>6.3463</v>
+      </c>
+      <c r="D264">
+        <v>6.3213</v>
+      </c>
+      <c r="E264">
+        <v>6.3331</v>
+      </c>
+      <c r="F264">
+        <v>3856.723215</v>
+      </c>
+      <c r="G264" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7">
+      <c r="A265" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B265" s="2">
+        <v>45519</v>
+      </c>
+      <c r="C265">
+        <v>5.6255</v>
+      </c>
+      <c r="D265">
+        <v>5.6019</v>
+      </c>
+      <c r="E265">
+        <v>5.6131</v>
+      </c>
+      <c r="F265">
+        <v>3847.093173</v>
+      </c>
+      <c r="G265" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7">
+      <c r="A266" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B266" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C266">
+        <v>5.4531</v>
+      </c>
+      <c r="D266">
+        <v>5.4281</v>
+      </c>
+      <c r="E266">
+        <v>5.44</v>
+      </c>
+      <c r="F266">
+        <v>3932.570752</v>
+      </c>
+      <c r="G266" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="A267" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B267" s="2">
+        <v>46249</v>
+      </c>
+      <c r="C267">
+        <v>5.3238</v>
+      </c>
+      <c r="D267">
+        <v>5.2996</v>
+      </c>
+      <c r="E267">
+        <v>5.31</v>
+      </c>
+      <c r="F267">
+        <v>3914.56063</v>
+      </c>
+      <c r="G267" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7">
+      <c r="A268" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B268" s="2">
+        <v>46522</v>
+      </c>
+      <c r="C268">
+        <v>5.3773</v>
+      </c>
+      <c r="D268">
+        <v>5.3525</v>
+      </c>
+      <c r="E268">
+        <v>5.365</v>
+      </c>
+      <c r="F268">
+        <v>3977.942845</v>
+      </c>
+      <c r="G268" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7">
+      <c r="A269" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B269" s="2">
+        <v>46980</v>
+      </c>
+      <c r="C269">
+        <v>5.4575</v>
+      </c>
+      <c r="D269">
+        <v>5.4312</v>
+      </c>
+      <c r="E269">
+        <v>5.4456</v>
+      </c>
+      <c r="F269">
+        <v>3926.595324</v>
+      </c>
+      <c r="G269" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7">
+      <c r="A270" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B270" s="2">
+        <v>47710</v>
+      </c>
+      <c r="C270">
+        <v>5.5476</v>
+      </c>
+      <c r="D270">
+        <v>5.5206</v>
+      </c>
+      <c r="E270">
+        <v>5.5325</v>
+      </c>
+      <c r="F270">
+        <v>3933.976959</v>
+      </c>
+      <c r="G270" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7">
+      <c r="A271" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B271" s="2">
+        <v>48441</v>
+      </c>
+      <c r="C271">
+        <v>5.5943</v>
+      </c>
+      <c r="D271">
+        <v>5.5613</v>
+      </c>
+      <c r="E271">
+        <v>5.58</v>
+      </c>
+      <c r="F271">
+        <v>3939.315973</v>
+      </c>
+      <c r="G271" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B272" s="2">
+        <v>49444</v>
+      </c>
+      <c r="C272">
+        <v>5.615</v>
+      </c>
+      <c r="D272">
+        <v>5.5871</v>
+      </c>
+      <c r="E272">
+        <v>5.6</v>
+      </c>
+      <c r="F272">
+        <v>4013.391461</v>
+      </c>
+      <c r="G272" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B273" s="2">
+        <v>51363</v>
+      </c>
+      <c r="C273">
+        <v>5.669</v>
+      </c>
+      <c r="D273">
+        <v>5.6229</v>
+      </c>
+      <c r="E273">
+        <v>5.6442</v>
+      </c>
+      <c r="F273">
+        <v>3970.42402</v>
+      </c>
+      <c r="G273" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B274" s="2">
+        <v>53097</v>
+      </c>
+      <c r="C274">
+        <v>5.7245</v>
+      </c>
+      <c r="D274">
+        <v>5.6831</v>
+      </c>
+      <c r="E274">
+        <v>5.7056</v>
+      </c>
+      <c r="F274">
+        <v>4018.04452</v>
+      </c>
+      <c r="G274" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7">
+      <c r="A275" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B275" s="2">
+        <v>55015</v>
+      </c>
+      <c r="C275">
+        <v>5.7304</v>
+      </c>
+      <c r="D275">
+        <v>5.6948</v>
+      </c>
+      <c r="E275">
+        <v>5.7134</v>
+      </c>
+      <c r="F275">
+        <v>3971.506304</v>
+      </c>
+      <c r="G275" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="A276" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B276" s="2">
+        <v>56749</v>
+      </c>
+      <c r="C276">
+        <v>5.7083</v>
+      </c>
+      <c r="D276">
+        <v>5.6781</v>
+      </c>
+      <c r="E276">
+        <v>5.6936</v>
+      </c>
+      <c r="F276">
+        <v>4049.205918</v>
+      </c>
+      <c r="G276" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7">
+      <c r="A277" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B277" s="2">
+        <v>58668</v>
+      </c>
+      <c r="C277">
+        <v>5.7092</v>
+      </c>
+      <c r="D277">
+        <v>5.6762</v>
+      </c>
+      <c r="E277">
+        <v>5.6921</v>
+      </c>
+      <c r="F277">
+        <v>4001.77215</v>
+      </c>
+      <c r="G277" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>